<commit_message>
added notes for free exploration
</commit_message>
<xml_diff>
--- a/Testmethoden/Heuristik Walkthrough/Walkthrough Ben.xlsx
+++ b/Testmethoden/Heuristik Walkthrough/Walkthrough Ben.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
   <si>
     <t>Szenario </t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Task nicht lösbar?</t>
+  </si>
+  <si>
+    <t>In “Berichte Studiengebühren” sind keine Berichte?</t>
+  </si>
+  <si>
+    <t>“Newsletter” in “Newsletter (Rzettel)” umbenennen wegen Branding</t>
   </si>
 </sst>
 </file>
@@ -280,10 +286,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -477,6 +483,28 @@
       </c>
       <c r="D16" s="10"/>
     </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>